<commit_message>
Add .gitignore to ignore pycache and p file; add green phase prediction in intersectionpy; add four types of vehicles
</commit_message>
<xml_diff>
--- a/4x4-run-data-rule-ppo-TSC-train-phase_stability_in_reward-limited_cycle_120-more_layers.xlsx
+++ b/4x4-run-data-rule-ppo-TSC-train-phase_stability_in_reward-limited_cycle_120-more_layers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AP1"/>
+  <dimension ref="A1:BA1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,190 +456,245 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>avg_speed_car</t>
+          <t>avg_speed_icev</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>energy_per_mile_car</t>
+          <t>energy_per_mile_icev</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>avg_veh_num_car</t>
+          <t>avg_veh_num_icev</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>avg_speed_ev</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>energy_per_mile_ev</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>avg_veh_num_ev</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>avg_speed_cav</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>energy_per_mile_cav</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>avg_veh_num_cav</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>avg_speed_caev</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>energy_per_mile_caev</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>avg_veh_num_caev</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
           <t>Ep_num_train_rollouts</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Ep_rollout_length</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Ep_eval_freq</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Ep_eval_num_eps</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Ep_max_ep_steps</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Ep_generation_ep_steps</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Ep_warmup_ep_steps</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Ep_test_num_eps</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>A_agent_type</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>A_single_agent</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>P_gae_tau</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>P_entropy_weight</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>P_minibatch_size</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>P_optimization_epochs</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>P_ppo_ratio_clip</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>P_discount</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>P_learning_rate</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>P_clip_grads</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>P_gradient_clip</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>P_value_loss_coef</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>P_hidden_layer_size</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>P_actor_layer_size</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>P_critic_layer_size</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>R_rule_set</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>R_rule_set_params</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>En_shape</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>En_rush_hour</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>En_uniform_generation_probability</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>En_use_vehicle_controller</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>En_step_length</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>En_gather_vehicle_info</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>En_actuated_tls</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>En_phase_mode</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>En_vehicle_type_distribution</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>M_reward_interpolation</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>M_state_interpolation</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>P_num_workers</t>
         </is>

</xml_diff>